<commit_message>
Updated Weekly Reports and Timesheet Tracking.
Reviewed weekly reports and timesheets for Summer Week 2. Updated the
spreadsheets accordingly.
Uploaded timesheet for week 2 and weekly report.
</commit_message>
<xml_diff>
--- a/Documents/Management/Reports and Timesheets Tracking.xlsx
+++ b/Documents/Management/Reports and Timesheets Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Checklists" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="32">
   <si>
     <t>Weekly Reports Checklist</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Term</t>
+  </si>
+  <si>
+    <t>dates?</t>
+  </si>
+  <si>
+    <t>detail?</t>
   </si>
 </sst>
 </file>
@@ -215,8 +221,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -311,6 +335,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -320,17 +353,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="93">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -368,6 +392,15 @@
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -405,6 +438,15 @@
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -745,7 +787,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -820,7 +862,7 @@
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="7">
@@ -847,7 +889,7 @@
       <c r="J7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="14" t="s">
         <v>20</v>
       </c>
       <c r="L7" s="2" t="s">
@@ -858,7 +900,7 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="13"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="7">
         <v>10</v>
       </c>
@@ -871,7 +913,7 @@
       <c r="F8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="12" t="s">
         <v>15</v>
       </c>
       <c r="H8" s="4" t="s">
@@ -883,8 +925,8 @@
       <c r="J8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17" t="s">
+      <c r="K8" s="14"/>
+      <c r="L8" s="14" t="s">
         <v>19</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -892,7 +934,7 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="7">
@@ -907,7 +949,7 @@
       <c r="F9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="4" t="s">
         <v>13</v>
       </c>
@@ -917,14 +959,14 @@
       <c r="J9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
       <c r="M9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="B10" s="13"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="7">
         <v>2</v>
       </c>
@@ -937,7 +979,7 @@
       <c r="F10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="4" t="s">
@@ -949,14 +991,14 @@
       <c r="J10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
       <c r="M10" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="B11" s="13"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="7">
         <v>3</v>
       </c>
@@ -969,7 +1011,7 @@
       <c r="F11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="16"/>
+      <c r="G11" s="13"/>
       <c r="H11" s="4" t="s">
         <v>13</v>
       </c>
@@ -979,14 +1021,14 @@
       <c r="J11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
       <c r="M11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="B12" s="13"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="7">
         <v>4</v>
       </c>
@@ -999,22 +1041,24 @@
       <c r="F12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="16"/>
+      <c r="G12" s="13"/>
       <c r="H12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="15" t="s">
+      <c r="J12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="B13" s="13"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="7">
         <v>5</v>
       </c>
@@ -1036,13 +1080,13 @@
       <c r="I13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="15"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="16" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="7">
@@ -1057,32 +1101,62 @@
       <c r="F14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="G14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="13"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="B15" s="13"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="7">
         <v>2</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
+      <c r="D15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="B16" s="13"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="7">
         <v>3</v>
       </c>
@@ -1098,7 +1172,7 @@
       <c r="M16" s="10"/>
     </row>
     <row r="17" spans="2:13">
-      <c r="B17" s="13"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="7">
         <v>4</v>
       </c>
@@ -1114,7 +1188,7 @@
       <c r="M17" s="10"/>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="13"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="7">
         <v>5</v>
       </c>
@@ -1130,7 +1204,7 @@
       <c r="M18" s="10"/>
     </row>
     <row r="19" spans="2:13">
-      <c r="B19" s="13"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="7">
         <v>6</v>
       </c>
@@ -1146,7 +1220,7 @@
       <c r="M19" s="10"/>
     </row>
     <row r="20" spans="2:13">
-      <c r="B20" s="13"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="7">
         <v>7</v>
       </c>
@@ -1162,7 +1236,7 @@
       <c r="M20" s="10"/>
     </row>
     <row r="21" spans="2:13">
-      <c r="B21" s="13"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="7">
         <v>8</v>
       </c>
@@ -1192,10 +1266,10 @@
       </c>
     </row>
     <row r="27" spans="2:13">
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="14"/>
+      <c r="C27" s="17"/>
       <c r="D27" s="1" t="s">
         <v>2</v>
       </c>
@@ -1228,7 +1302,7 @@
       </c>
     </row>
     <row r="28" spans="2:13">
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="7">
@@ -1246,7 +1320,7 @@
       <c r="M28" s="10"/>
     </row>
     <row r="29" spans="2:13">
-      <c r="B29" s="13"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="7">
         <v>2</v>
       </c>
@@ -1280,7 +1354,7 @@
       </c>
     </row>
     <row r="30" spans="2:13">
-      <c r="B30" s="13"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="7">
         <v>3</v>
       </c>
@@ -1316,7 +1390,7 @@
       </c>
     </row>
     <row r="31" spans="2:13">
-      <c r="B31" s="13"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="7">
         <v>4</v>
       </c>
@@ -1352,7 +1426,7 @@
       </c>
     </row>
     <row r="32" spans="2:13">
-      <c r="B32" s="13"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="7">
         <v>5</v>
       </c>
@@ -1388,7 +1462,7 @@
       </c>
     </row>
     <row r="33" spans="2:13">
-      <c r="B33" s="13"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="7">
         <v>6</v>
       </c>
@@ -1424,7 +1498,7 @@
       </c>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="13"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="7">
         <v>7</v>
       </c>
@@ -1460,7 +1534,7 @@
       </c>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="13"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="7">
         <v>8</v>
       </c>
@@ -1496,7 +1570,7 @@
       </c>
     </row>
     <row r="36" spans="2:13">
-      <c r="B36" s="13"/>
+      <c r="B36" s="16"/>
       <c r="C36" s="7">
         <v>9</v>
       </c>
@@ -1532,7 +1606,7 @@
       </c>
     </row>
     <row r="37" spans="2:13">
-      <c r="B37" s="13"/>
+      <c r="B37" s="16"/>
       <c r="C37" s="7">
         <v>10</v>
       </c>
@@ -1568,7 +1642,7 @@
       </c>
     </row>
     <row r="38" spans="2:13">
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C38" s="9">
@@ -1606,7 +1680,7 @@
       </c>
     </row>
     <row r="39" spans="2:13">
-      <c r="B39" s="12"/>
+      <c r="B39" s="15"/>
       <c r="C39" s="9">
         <v>2</v>
       </c>
@@ -1642,7 +1716,7 @@
       </c>
     </row>
     <row r="40" spans="2:13">
-      <c r="B40" s="12"/>
+      <c r="B40" s="15"/>
       <c r="C40" s="9">
         <v>3</v>
       </c>
@@ -1678,7 +1752,7 @@
       </c>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" s="12"/>
+      <c r="B41" s="15"/>
       <c r="C41" s="9">
         <v>4</v>
       </c>
@@ -1714,7 +1788,7 @@
       </c>
     </row>
     <row r="42" spans="2:13">
-      <c r="B42" s="12"/>
+      <c r="B42" s="15"/>
       <c r="C42" s="9">
         <v>5</v>
       </c>
@@ -1750,7 +1824,7 @@
       </c>
     </row>
     <row r="43" spans="2:13">
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C43" s="9">
@@ -1780,29 +1854,51 @@
       <c r="K43" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="L43" s="3"/>
+      <c r="L43" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="M43" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="44" spans="2:13">
-      <c r="B44" s="12"/>
+      <c r="B44" s="15"/>
       <c r="C44" s="9">
         <v>2</v>
       </c>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="10"/>
-      <c r="K44" s="10"/>
-      <c r="L44" s="10"/>
-      <c r="M44" s="10"/>
+      <c r="D44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M44" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="45" spans="2:13">
-      <c r="B45" s="12"/>
+      <c r="B45" s="15"/>
       <c r="C45" s="9">
         <v>3</v>
       </c>
@@ -1818,7 +1914,7 @@
       <c r="M45" s="10"/>
     </row>
     <row r="46" spans="2:13">
-      <c r="B46" s="12"/>
+      <c r="B46" s="15"/>
       <c r="C46" s="9">
         <v>4</v>
       </c>
@@ -1834,7 +1930,7 @@
       <c r="M46" s="10"/>
     </row>
     <row r="47" spans="2:13">
-      <c r="B47" s="12"/>
+      <c r="B47" s="15"/>
       <c r="C47" s="9">
         <v>5</v>
       </c>
@@ -1850,7 +1946,7 @@
       <c r="M47" s="10"/>
     </row>
     <row r="48" spans="2:13">
-      <c r="B48" s="12"/>
+      <c r="B48" s="15"/>
       <c r="C48" s="9">
         <v>6</v>
       </c>
@@ -1866,7 +1962,7 @@
       <c r="M48" s="10"/>
     </row>
     <row r="49" spans="2:13">
-      <c r="B49" s="12"/>
+      <c r="B49" s="15"/>
       <c r="C49" s="9">
         <v>7</v>
       </c>
@@ -1882,7 +1978,7 @@
       <c r="M49" s="10"/>
     </row>
     <row r="50" spans="2:13">
-      <c r="B50" s="12"/>
+      <c r="B50" s="15"/>
       <c r="C50" s="9">
         <v>8</v>
       </c>
@@ -1901,12 +1997,7 @@
   <sortState ref="D4:M4">
     <sortCondition ref="D4"/>
   </sortState>
-  <mergeCells count="12">
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="K7:K14"/>
-    <mergeCell ref="L8:L13"/>
-    <mergeCell ref="M12:M13"/>
+  <mergeCells count="13">
     <mergeCell ref="B38:B42"/>
     <mergeCell ref="B43:B50"/>
     <mergeCell ref="B28:B37"/>
@@ -1914,6 +2005,12 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B14:B21"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="K7:K14"/>
+    <mergeCell ref="L8:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="J12:J14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated Weekly Report and Timesheet Documents
Uploaded weekly report and timesheet for week 4.
Renamed AG’s week 4 report (wrong date).
Updated tracking spreadsheets.
</commit_message>
<xml_diff>
--- a/Documents/Management/Reports and Timesheets Tracking.xlsx
+++ b/Documents/Management/Reports and Timesheets Tracking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="34">
   <si>
     <t>Weekly Reports Checklist</t>
   </si>
@@ -237,8 +237,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="135">
+  <cellStyleXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -392,6 +432,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -401,19 +452,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="135">
+  <cellStyles count="175">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -481,6 +521,26 @@
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -548,6 +608,26 @@
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -888,7 +968,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -920,7 +1000,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="4">
-        <v>41772</v>
+        <v>41779</v>
       </c>
       <c r="N4" s="1"/>
     </row>
@@ -963,7 +1043,7 @@
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="6">
@@ -990,7 +1070,7 @@
       <c r="J7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="K7" s="15" t="s">
         <v>20</v>
       </c>
       <c r="L7" s="2" t="s">
@@ -1001,7 +1081,7 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="12"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="6">
         <v>10</v>
       </c>
@@ -1026,8 +1106,8 @@
       <c r="J8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16" t="s">
+      <c r="K8" s="15"/>
+      <c r="L8" s="15" t="s">
         <v>19</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -1035,7 +1115,7 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="17" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="6">
@@ -1060,14 +1140,14 @@
       <c r="J9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
       <c r="M9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="B10" s="12"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="6">
         <v>2</v>
       </c>
@@ -1080,7 +1160,7 @@
       <c r="F10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="3" t="s">
@@ -1092,14 +1172,14 @@
       <c r="J10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
       <c r="M10" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="B11" s="12"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="6">
         <v>3</v>
       </c>
@@ -1112,7 +1192,7 @@
       <c r="F11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="15"/>
+      <c r="G11" s="13"/>
       <c r="H11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1122,14 +1202,14 @@
       <c r="J11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
       <c r="M11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="B12" s="12"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="6">
         <v>4</v>
       </c>
@@ -1142,24 +1222,24 @@
       <c r="F12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="13"/>
       <c r="H12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="15" t="s">
+      <c r="J12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
       <c r="M12" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="B13" s="12"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="6">
         <v>5</v>
       </c>
@@ -1181,13 +1261,13 @@
       <c r="I13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="15"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
       <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="17" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="6">
@@ -1211,8 +1291,8 @@
       <c r="I14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="16"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="15"/>
       <c r="L14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1221,7 +1301,7 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="B15" s="12"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="6">
         <v>2</v>
       </c>
@@ -1243,7 +1323,7 @@
       <c r="I15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J15" s="15" t="s">
+      <c r="J15" s="13" t="s">
         <v>30</v>
       </c>
       <c r="K15" s="3" t="s">
@@ -1257,7 +1337,7 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="B16" s="12"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="6">
         <v>3</v>
       </c>
@@ -1270,44 +1350,64 @@
       <c r="F16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="13"/>
+      <c r="K16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J16" s="15"/>
-      <c r="K16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L16" s="17" t="s">
-        <v>32</v>
-      </c>
       <c r="M16" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="2:13">
-      <c r="B17" s="12"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="6">
         <v>4</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
+      <c r="D17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="12"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="6">
         <v>5</v>
       </c>
@@ -1323,7 +1423,7 @@
       <c r="M18" s="9"/>
     </row>
     <row r="19" spans="2:13">
-      <c r="B19" s="12"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="6">
         <v>6</v>
       </c>
@@ -1339,7 +1439,7 @@
       <c r="M19" s="9"/>
     </row>
     <row r="20" spans="2:13">
-      <c r="B20" s="12"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="6">
         <v>7</v>
       </c>
@@ -1355,7 +1455,7 @@
       <c r="M20" s="9"/>
     </row>
     <row r="21" spans="2:13">
-      <c r="B21" s="12"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="6">
         <v>8</v>
       </c>
@@ -1381,14 +1481,14 @@
         <v>24</v>
       </c>
       <c r="C25" s="4">
-        <v>41772</v>
+        <v>41779</v>
       </c>
     </row>
     <row r="27" spans="2:13">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="13"/>
+      <c r="C27" s="18"/>
       <c r="D27" s="1" t="s">
         <v>2</v>
       </c>
@@ -1421,7 +1521,7 @@
       </c>
     </row>
     <row r="28" spans="2:13">
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="6">
@@ -1439,7 +1539,7 @@
       <c r="M28" s="9"/>
     </row>
     <row r="29" spans="2:13">
-      <c r="B29" s="12"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="6">
         <v>2</v>
       </c>
@@ -1464,7 +1564,7 @@
       <c r="J29" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K29" s="17" t="s">
+      <c r="K29" s="11" t="s">
         <v>32</v>
       </c>
       <c r="L29" s="3" t="s">
@@ -1475,7 +1575,7 @@
       </c>
     </row>
     <row r="30" spans="2:13">
-      <c r="B30" s="12"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="6">
         <v>3</v>
       </c>
@@ -1511,7 +1611,7 @@
       </c>
     </row>
     <row r="31" spans="2:13">
-      <c r="B31" s="12"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="6">
         <v>4</v>
       </c>
@@ -1547,7 +1647,7 @@
       </c>
     </row>
     <row r="32" spans="2:13">
-      <c r="B32" s="12"/>
+      <c r="B32" s="17"/>
       <c r="C32" s="6">
         <v>5</v>
       </c>
@@ -1583,7 +1683,7 @@
       </c>
     </row>
     <row r="33" spans="2:13">
-      <c r="B33" s="12"/>
+      <c r="B33" s="17"/>
       <c r="C33" s="6">
         <v>6</v>
       </c>
@@ -1619,7 +1719,7 @@
       </c>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="12"/>
+      <c r="B34" s="17"/>
       <c r="C34" s="6">
         <v>7</v>
       </c>
@@ -1655,7 +1755,7 @@
       </c>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="12"/>
+      <c r="B35" s="17"/>
       <c r="C35" s="6">
         <v>8</v>
       </c>
@@ -1691,7 +1791,7 @@
       </c>
     </row>
     <row r="36" spans="2:13">
-      <c r="B36" s="12"/>
+      <c r="B36" s="17"/>
       <c r="C36" s="6">
         <v>9</v>
       </c>
@@ -1727,7 +1827,7 @@
       </c>
     </row>
     <row r="37" spans="2:13">
-      <c r="B37" s="12"/>
+      <c r="B37" s="17"/>
       <c r="C37" s="6">
         <v>10</v>
       </c>
@@ -1763,7 +1863,7 @@
       </c>
     </row>
     <row r="38" spans="2:13">
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C38" s="8">
@@ -1801,7 +1901,7 @@
       </c>
     </row>
     <row r="39" spans="2:13">
-      <c r="B39" s="11"/>
+      <c r="B39" s="16"/>
       <c r="C39" s="8">
         <v>2</v>
       </c>
@@ -1837,7 +1937,7 @@
       </c>
     </row>
     <row r="40" spans="2:13">
-      <c r="B40" s="11"/>
+      <c r="B40" s="16"/>
       <c r="C40" s="8">
         <v>3</v>
       </c>
@@ -1873,7 +1973,7 @@
       </c>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" s="11"/>
+      <c r="B41" s="16"/>
       <c r="C41" s="8">
         <v>4</v>
       </c>
@@ -1909,7 +2009,7 @@
       </c>
     </row>
     <row r="42" spans="2:13">
-      <c r="B42" s="11"/>
+      <c r="B42" s="16"/>
       <c r="C42" s="8">
         <v>5</v>
       </c>
@@ -1945,7 +2045,7 @@
       </c>
     </row>
     <row r="43" spans="2:13">
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="16" t="s">
         <v>28</v>
       </c>
       <c r="C43" s="8">
@@ -1983,7 +2083,7 @@
       </c>
     </row>
     <row r="44" spans="2:13">
-      <c r="B44" s="11"/>
+      <c r="B44" s="16"/>
       <c r="C44" s="8">
         <v>2</v>
       </c>
@@ -2019,7 +2119,7 @@
       </c>
     </row>
     <row r="45" spans="2:13">
-      <c r="B45" s="11"/>
+      <c r="B45" s="16"/>
       <c r="C45" s="8">
         <v>3</v>
       </c>
@@ -2032,46 +2132,66 @@
       <c r="F45" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G45" s="17" t="s">
+      <c r="G45" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K45" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L45" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H45" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J45" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="K45" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="L45" s="17" t="s">
-        <v>32</v>
-      </c>
       <c r="M45" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="46" spans="2:13">
-      <c r="B46" s="11"/>
+      <c r="B46" s="16"/>
       <c r="C46" s="8">
         <v>4</v>
       </c>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
+      <c r="D46" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J46" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K46" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L46" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="47" spans="2:13">
-      <c r="B47" s="11"/>
+      <c r="B47" s="16"/>
       <c r="C47" s="8">
         <v>5</v>
       </c>
@@ -2087,7 +2207,7 @@
       <c r="M47" s="9"/>
     </row>
     <row r="48" spans="2:13">
-      <c r="B48" s="11"/>
+      <c r="B48" s="16"/>
       <c r="C48" s="8">
         <v>6</v>
       </c>
@@ -2103,7 +2223,7 @@
       <c r="M48" s="9"/>
     </row>
     <row r="49" spans="2:13">
-      <c r="B49" s="11"/>
+      <c r="B49" s="16"/>
       <c r="C49" s="8">
         <v>7</v>
       </c>
@@ -2119,7 +2239,7 @@
       <c r="M49" s="9"/>
     </row>
     <row r="50" spans="2:13">
-      <c r="B50" s="11"/>
+      <c r="B50" s="16"/>
       <c r="C50" s="8">
         <v>8</v>
       </c>
@@ -2139,20 +2259,20 @@
     <sortCondition ref="D4"/>
   </sortState>
   <mergeCells count="14">
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="K7:K14"/>
-    <mergeCell ref="L8:L13"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="B14:B21"/>
     <mergeCell ref="M12:M13"/>
     <mergeCell ref="J12:J14"/>
     <mergeCell ref="B38:B42"/>
     <mergeCell ref="B43:B50"/>
     <mergeCell ref="B28:B37"/>
     <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="K7:K14"/>
+    <mergeCell ref="L8:L13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Weekly review of reports and timesheets
Checked timesheets and reports for week 5.
Updated tracking spreadsheets.
</commit_message>
<xml_diff>
--- a/Documents/Management/Reports and Timesheets Tracking.xlsx
+++ b/Documents/Management/Reports and Timesheets Tracking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="34">
   <si>
     <t>Weekly Reports Checklist</t>
   </si>
@@ -133,7 +133,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -190,7 +189,7 @@
       <name val="Zapf Dingbats"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,6 +226,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -237,7 +242,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="175">
+  <cellStyleXfs count="247">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -413,8 +418,80 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -434,26 +511,27 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="175">
+  <cellStyles count="247">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -541,6 +619,42 @@
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -628,6 +742,42 @@
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -968,7 +1118,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1000,7 +1150,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="4">
-        <v>41779</v>
+        <v>41787</v>
       </c>
       <c r="N4" s="1"/>
     </row>
@@ -1043,7 +1193,7 @@
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="6">
@@ -1070,7 +1220,7 @@
       <c r="J7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="18" t="s">
         <v>20</v>
       </c>
       <c r="L7" s="2" t="s">
@@ -1081,7 +1231,7 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="17"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="6">
         <v>10</v>
       </c>
@@ -1106,8 +1256,8 @@
       <c r="J8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15" t="s">
+      <c r="K8" s="18"/>
+      <c r="L8" s="18" t="s">
         <v>19</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -1115,7 +1265,7 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="6">
@@ -1140,14 +1290,14 @@
       <c r="J9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
       <c r="M9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="B10" s="17"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="6">
         <v>2</v>
       </c>
@@ -1160,7 +1310,7 @@
       <c r="F10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="15" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="3" t="s">
@@ -1172,14 +1322,14 @@
       <c r="J10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
       <c r="M10" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="B11" s="17"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="6">
         <v>3</v>
       </c>
@@ -1192,7 +1342,7 @@
       <c r="F11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="13"/>
+      <c r="G11" s="15"/>
       <c r="H11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1202,14 +1352,14 @@
       <c r="J11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
       <c r="M11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="B12" s="17"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="6">
         <v>4</v>
       </c>
@@ -1222,24 +1372,24 @@
       <c r="F12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="13"/>
+      <c r="G12" s="15"/>
       <c r="H12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
       <c r="M12" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="B13" s="17"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="6">
         <v>5</v>
       </c>
@@ -1261,13 +1411,13 @@
       <c r="I13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
       <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="6">
@@ -1291,8 +1441,8 @@
       <c r="I14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="18"/>
       <c r="L14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1301,7 +1451,7 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="B15" s="17"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="6">
         <v>2</v>
       </c>
@@ -1323,7 +1473,7 @@
       <c r="I15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J15" s="13" t="s">
+      <c r="J15" s="15" t="s">
         <v>30</v>
       </c>
       <c r="K15" s="3" t="s">
@@ -1337,7 +1487,7 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="B16" s="17"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="6">
         <v>3</v>
       </c>
@@ -1359,7 +1509,7 @@
       <c r="I16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="13"/>
+      <c r="J16" s="15"/>
       <c r="K16" s="3" t="s">
         <v>13</v>
       </c>
@@ -1371,7 +1521,7 @@
       </c>
     </row>
     <row r="17" spans="2:13">
-      <c r="B17" s="17"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="6">
         <v>4</v>
       </c>
@@ -1390,14 +1540,14 @@
       <c r="H17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>32</v>
+      <c r="I17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="L17" s="11" t="s">
         <v>32</v>
@@ -1407,23 +1557,43 @@
       </c>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="17"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="6">
         <v>5</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
+      <c r="D18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M18" s="11" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" spans="2:13">
-      <c r="B19" s="17"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="6">
         <v>6</v>
       </c>
@@ -1439,7 +1609,7 @@
       <c r="M19" s="9"/>
     </row>
     <row r="20" spans="2:13">
-      <c r="B20" s="17"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="6">
         <v>7</v>
       </c>
@@ -1455,7 +1625,7 @@
       <c r="M20" s="9"/>
     </row>
     <row r="21" spans="2:13">
-      <c r="B21" s="17"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="6">
         <v>8</v>
       </c>
@@ -1481,14 +1651,14 @@
         <v>24</v>
       </c>
       <c r="C25" s="4">
-        <v>41779</v>
+        <v>41787</v>
       </c>
     </row>
     <row r="27" spans="2:13">
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="18"/>
+      <c r="C27" s="17"/>
       <c r="D27" s="1" t="s">
         <v>2</v>
       </c>
@@ -1521,7 +1691,7 @@
       </c>
     </row>
     <row r="28" spans="2:13">
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="6">
@@ -1539,7 +1709,7 @@
       <c r="M28" s="9"/>
     </row>
     <row r="29" spans="2:13">
-      <c r="B29" s="17"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="6">
         <v>2</v>
       </c>
@@ -1575,7 +1745,7 @@
       </c>
     </row>
     <row r="30" spans="2:13">
-      <c r="B30" s="17"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="6">
         <v>3</v>
       </c>
@@ -1611,7 +1781,7 @@
       </c>
     </row>
     <row r="31" spans="2:13">
-      <c r="B31" s="17"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="6">
         <v>4</v>
       </c>
@@ -1647,7 +1817,7 @@
       </c>
     </row>
     <row r="32" spans="2:13">
-      <c r="B32" s="17"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="6">
         <v>5</v>
       </c>
@@ -1683,7 +1853,7 @@
       </c>
     </row>
     <row r="33" spans="2:13">
-      <c r="B33" s="17"/>
+      <c r="B33" s="13"/>
       <c r="C33" s="6">
         <v>6</v>
       </c>
@@ -1719,7 +1889,7 @@
       </c>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="17"/>
+      <c r="B34" s="13"/>
       <c r="C34" s="6">
         <v>7</v>
       </c>
@@ -1755,7 +1925,7 @@
       </c>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="17"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="6">
         <v>8</v>
       </c>
@@ -1791,7 +1961,7 @@
       </c>
     </row>
     <row r="36" spans="2:13">
-      <c r="B36" s="17"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="6">
         <v>9</v>
       </c>
@@ -1827,7 +1997,7 @@
       </c>
     </row>
     <row r="37" spans="2:13">
-      <c r="B37" s="17"/>
+      <c r="B37" s="13"/>
       <c r="C37" s="6">
         <v>10</v>
       </c>
@@ -2147,8 +2317,8 @@
       <c r="K45" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="L45" s="11" t="s">
-        <v>32</v>
+      <c r="L45" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="M45" s="3" t="s">
         <v>13</v>
@@ -2174,17 +2344,17 @@
       <c r="H46" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I46" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="J46" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="K46" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="L46" s="11" t="s">
-        <v>32</v>
+      <c r="I46" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J46" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K46" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="M46" s="3" t="s">
         <v>13</v>
@@ -2195,16 +2365,36 @@
       <c r="C47" s="8">
         <v>5</v>
       </c>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
-      <c r="M47" s="9"/>
+      <c r="D47" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J47" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K47" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L47" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M47" s="19" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="48" spans="2:13">
       <c r="B48" s="16"/>
@@ -2259,16 +2449,16 @@
     <sortCondition ref="D4"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B43:B50"/>
+    <mergeCell ref="B28:B37"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="J15:J16"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B14:B21"/>
     <mergeCell ref="M12:M13"/>
     <mergeCell ref="J12:J14"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="B43:B50"/>
-    <mergeCell ref="B28:B37"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="J15:J16"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="G10:G12"/>
     <mergeCell ref="K7:K14"/>

</xml_diff>

<commit_message>
Reviewed Weekly Reports and Timesheets
Conducted review of week 6 reports and timesheets.
Updated tracking spreadsheets.
</commit_message>
<xml_diff>
--- a/Documents/Management/Reports and Timesheets Tracking.xlsx
+++ b/Documents/Management/Reports and Timesheets Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20360" windowHeight="21080" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20280" windowHeight="21080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Checklists" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="33">
   <si>
     <t>Weekly Reports Checklist</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>✖</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
 </sst>
 </file>
@@ -189,7 +186,7 @@
       <name val="Zapf Dingbats"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,12 +219,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
@@ -242,7 +233,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="247">
+  <cellStyleXfs count="319">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -490,8 +481,80 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -510,28 +573,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="247">
+  <cellStyles count="319">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -655,6 +717,42 @@
     <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -778,6 +876,42 @@
     <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1118,7 +1252,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1150,7 +1284,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="4">
-        <v>41787</v>
+        <v>41794</v>
       </c>
       <c r="N4" s="1"/>
     </row>
@@ -1193,7 +1327,7 @@
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="6">
@@ -1231,7 +1365,7 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="13"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="6">
         <v>10</v>
       </c>
@@ -1244,7 +1378,7 @@
       <c r="F8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="17" t="s">
         <v>15</v>
       </c>
       <c r="H8" s="3" t="s">
@@ -1265,7 +1399,7 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="6">
@@ -1280,7 +1414,7 @@
       <c r="F9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="14"/>
+      <c r="G9" s="17"/>
       <c r="H9" s="3" t="s">
         <v>13</v>
       </c>
@@ -1297,7 +1431,7 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="B10" s="13"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="6">
         <v>2</v>
       </c>
@@ -1310,7 +1444,7 @@
       <c r="F10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="16" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="3" t="s">
@@ -1329,7 +1463,7 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="B11" s="13"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="6">
         <v>3</v>
       </c>
@@ -1342,7 +1476,7 @@
       <c r="F11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="15"/>
+      <c r="G11" s="16"/>
       <c r="H11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1359,7 +1493,7 @@
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="B12" s="13"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="6">
         <v>4</v>
       </c>
@@ -1372,24 +1506,24 @@
       <c r="F12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="16"/>
       <c r="H12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="15" t="s">
+      <c r="J12" s="16" t="s">
         <v>30</v>
       </c>
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
-      <c r="M12" s="14" t="s">
+      <c r="M12" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="B13" s="13"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="6">
         <v>5</v>
       </c>
@@ -1411,13 +1545,13 @@
       <c r="I13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="15"/>
+      <c r="J13" s="16"/>
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
-      <c r="M13" s="14"/>
+      <c r="M13" s="17"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="6">
@@ -1441,7 +1575,7 @@
       <c r="I14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="15"/>
+      <c r="J14" s="16"/>
       <c r="K14" s="18"/>
       <c r="L14" s="3" t="s">
         <v>13</v>
@@ -1451,7 +1585,7 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="B15" s="13"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="6">
         <v>2</v>
       </c>
@@ -1473,7 +1607,7 @@
       <c r="I15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J15" s="15" t="s">
+      <c r="J15" s="16" t="s">
         <v>30</v>
       </c>
       <c r="K15" s="3" t="s">
@@ -1487,7 +1621,7 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="B16" s="13"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="6">
         <v>3</v>
       </c>
@@ -1509,7 +1643,7 @@
       <c r="I16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="15"/>
+      <c r="J16" s="16"/>
       <c r="K16" s="3" t="s">
         <v>13</v>
       </c>
@@ -1521,7 +1655,7 @@
       </c>
     </row>
     <row r="17" spans="2:13">
-      <c r="B17" s="13"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="6">
         <v>4</v>
       </c>
@@ -1543,8 +1677,8 @@
       <c r="I17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="3" t="s">
-        <v>13</v>
+      <c r="J17" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>13</v>
@@ -1557,7 +1691,7 @@
       </c>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="13"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="6">
         <v>5</v>
       </c>
@@ -1576,11 +1710,11 @@
       <c r="H18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>32</v>
+      <c r="I18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>13</v>
@@ -1593,23 +1727,43 @@
       </c>
     </row>
     <row r="19" spans="2:13">
-      <c r="B19" s="13"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="6">
         <v>6</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
+      <c r="D19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M19" s="11" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" spans="2:13">
-      <c r="B20" s="13"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="6">
         <v>7</v>
       </c>
@@ -1625,7 +1779,7 @@
       <c r="M20" s="9"/>
     </row>
     <row r="21" spans="2:13">
-      <c r="B21" s="13"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="6">
         <v>8</v>
       </c>
@@ -1651,14 +1805,14 @@
         <v>24</v>
       </c>
       <c r="C25" s="4">
-        <v>41787</v>
+        <v>41794</v>
       </c>
     </row>
     <row r="27" spans="2:13">
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="17"/>
+      <c r="C27" s="15"/>
       <c r="D27" s="1" t="s">
         <v>2</v>
       </c>
@@ -1691,7 +1845,7 @@
       </c>
     </row>
     <row r="28" spans="2:13">
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="6">
@@ -1709,7 +1863,7 @@
       <c r="M28" s="9"/>
     </row>
     <row r="29" spans="2:13">
-      <c r="B29" s="13"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="6">
         <v>2</v>
       </c>
@@ -1745,7 +1899,7 @@
       </c>
     </row>
     <row r="30" spans="2:13">
-      <c r="B30" s="13"/>
+      <c r="B30" s="14"/>
       <c r="C30" s="6">
         <v>3</v>
       </c>
@@ -1781,7 +1935,7 @@
       </c>
     </row>
     <row r="31" spans="2:13">
-      <c r="B31" s="13"/>
+      <c r="B31" s="14"/>
       <c r="C31" s="6">
         <v>4</v>
       </c>
@@ -1817,7 +1971,7 @@
       </c>
     </row>
     <row r="32" spans="2:13">
-      <c r="B32" s="13"/>
+      <c r="B32" s="14"/>
       <c r="C32" s="6">
         <v>5</v>
       </c>
@@ -1853,7 +2007,7 @@
       </c>
     </row>
     <row r="33" spans="2:13">
-      <c r="B33" s="13"/>
+      <c r="B33" s="14"/>
       <c r="C33" s="6">
         <v>6</v>
       </c>
@@ -1889,7 +2043,7 @@
       </c>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="13"/>
+      <c r="B34" s="14"/>
       <c r="C34" s="6">
         <v>7</v>
       </c>
@@ -1925,7 +2079,7 @@
       </c>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="13"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="6">
         <v>8</v>
       </c>
@@ -1961,7 +2115,7 @@
       </c>
     </row>
     <row r="36" spans="2:13">
-      <c r="B36" s="13"/>
+      <c r="B36" s="14"/>
       <c r="C36" s="6">
         <v>9</v>
       </c>
@@ -1997,7 +2151,7 @@
       </c>
     </row>
     <row r="37" spans="2:13">
-      <c r="B37" s="13"/>
+      <c r="B37" s="14"/>
       <c r="C37" s="6">
         <v>10</v>
       </c>
@@ -2033,7 +2187,7 @@
       </c>
     </row>
     <row r="38" spans="2:13">
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C38" s="8">
@@ -2071,7 +2225,7 @@
       </c>
     </row>
     <row r="39" spans="2:13">
-      <c r="B39" s="16"/>
+      <c r="B39" s="13"/>
       <c r="C39" s="8">
         <v>2</v>
       </c>
@@ -2107,7 +2261,7 @@
       </c>
     </row>
     <row r="40" spans="2:13">
-      <c r="B40" s="16"/>
+      <c r="B40" s="13"/>
       <c r="C40" s="8">
         <v>3</v>
       </c>
@@ -2143,7 +2297,7 @@
       </c>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" s="16"/>
+      <c r="B41" s="13"/>
       <c r="C41" s="8">
         <v>4</v>
       </c>
@@ -2179,7 +2333,7 @@
       </c>
     </row>
     <row r="42" spans="2:13">
-      <c r="B42" s="16"/>
+      <c r="B42" s="13"/>
       <c r="C42" s="8">
         <v>5</v>
       </c>
@@ -2215,7 +2369,7 @@
       </c>
     </row>
     <row r="43" spans="2:13">
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C43" s="8">
@@ -2253,7 +2407,7 @@
       </c>
     </row>
     <row r="44" spans="2:13">
-      <c r="B44" s="16"/>
+      <c r="B44" s="13"/>
       <c r="C44" s="8">
         <v>2</v>
       </c>
@@ -2289,7 +2443,7 @@
       </c>
     </row>
     <row r="45" spans="2:13">
-      <c r="B45" s="16"/>
+      <c r="B45" s="13"/>
       <c r="C45" s="8">
         <v>3</v>
       </c>
@@ -2314,8 +2468,8 @@
       <c r="J45" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="K45" s="12" t="s">
-        <v>33</v>
+      <c r="K45" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="L45" s="3" t="s">
         <v>13</v>
@@ -2325,7 +2479,7 @@
       </c>
     </row>
     <row r="46" spans="2:13">
-      <c r="B46" s="16"/>
+      <c r="B46" s="13"/>
       <c r="C46" s="8">
         <v>4</v>
       </c>
@@ -2361,7 +2515,7 @@
       </c>
     </row>
     <row r="47" spans="2:13">
-      <c r="B47" s="16"/>
+      <c r="B47" s="13"/>
       <c r="C47" s="8">
         <v>5</v>
       </c>
@@ -2374,14 +2528,14 @@
       <c r="F47" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G47" s="11" t="s">
-        <v>32</v>
+      <c r="G47" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="H47" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I47" s="11" t="s">
-        <v>32</v>
+      <c r="I47" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="J47" s="10" t="s">
         <v>13</v>
@@ -2392,28 +2546,48 @@
       <c r="L47" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M47" s="19" t="s">
-        <v>32</v>
+      <c r="M47" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="2:13">
-      <c r="B48" s="16"/>
+      <c r="B48" s="13"/>
       <c r="C48" s="8">
         <v>6</v>
       </c>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
-      <c r="L48" s="9"/>
-      <c r="M48" s="9"/>
+      <c r="D48" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I48" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J48" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K48" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L48" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="M48" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="49" spans="2:13">
-      <c r="B49" s="16"/>
+      <c r="B49" s="13"/>
       <c r="C49" s="8">
         <v>7</v>
       </c>
@@ -2429,7 +2603,7 @@
       <c r="M49" s="9"/>
     </row>
     <row r="50" spans="2:13">
-      <c r="B50" s="16"/>
+      <c r="B50" s="13"/>
       <c r="C50" s="8">
         <v>8</v>
       </c>
@@ -2449,11 +2623,6 @@
     <sortCondition ref="D4"/>
   </sortState>
   <mergeCells count="14">
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="B43:B50"/>
-    <mergeCell ref="B28:B37"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="J15:J16"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B14:B21"/>
@@ -2463,6 +2632,11 @@
     <mergeCell ref="G10:G12"/>
     <mergeCell ref="K7:K14"/>
     <mergeCell ref="L8:L13"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B43:B50"/>
+    <mergeCell ref="B28:B37"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="J15:J16"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Worked on HTML Tour and Prepared Documentation
New folders. New PDFs.
Work on Software page is complete.
Tidied up some files.
</commit_message>
<xml_diff>
--- a/Documents/Management/Reports and Timesheets Tracking.xlsx
+++ b/Documents/Management/Reports and Timesheets Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20280" windowHeight="21080" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18140" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Checklists" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="34">
   <si>
     <t>Weekly Reports Checklist</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>✖</t>
+  </si>
+  <si>
+    <t>4 weeks late</t>
   </si>
 </sst>
 </file>
@@ -186,7 +189,7 @@
       <name val="Zapf Dingbats"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,12 +220,6 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -233,7 +230,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="319">
+  <cellStyleXfs count="359">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -553,8 +550,48 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -573,27 +610,39 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="319">
+  <cellStyles count="359">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -753,6 +802,26 @@
     <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -912,6 +981,26 @@
     <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1252,7 +1341,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1284,7 +1373,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="4">
-        <v>41794</v>
+        <v>41802</v>
       </c>
       <c r="N4" s="1"/>
     </row>
@@ -1327,7 +1416,7 @@
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="6">
@@ -1354,7 +1443,7 @@
       <c r="J7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="15" t="s">
         <v>20</v>
       </c>
       <c r="L7" s="2" t="s">
@@ -1365,7 +1454,7 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="14"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="6">
         <v>10</v>
       </c>
@@ -1378,7 +1467,7 @@
       <c r="F8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="13" t="s">
         <v>15</v>
       </c>
       <c r="H8" s="3" t="s">
@@ -1390,8 +1479,8 @@
       <c r="J8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18" t="s">
+      <c r="K8" s="15"/>
+      <c r="L8" s="15" t="s">
         <v>19</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -1399,7 +1488,7 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="6">
@@ -1414,7 +1503,7 @@
       <c r="F9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="17"/>
+      <c r="G9" s="13"/>
       <c r="H9" s="3" t="s">
         <v>13</v>
       </c>
@@ -1424,14 +1513,14 @@
       <c r="J9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
       <c r="M9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="B10" s="14"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="6">
         <v>2</v>
       </c>
@@ -1444,7 +1533,7 @@
       <c r="F10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="14" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="3" t="s">
@@ -1456,14 +1545,14 @@
       <c r="J10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
       <c r="M10" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="B11" s="14"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="6">
         <v>3</v>
       </c>
@@ -1476,7 +1565,7 @@
       <c r="F11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="16"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1486,14 +1575,14 @@
       <c r="J11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
       <c r="M11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="B12" s="14"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="6">
         <v>4</v>
       </c>
@@ -1506,24 +1595,24 @@
       <c r="F12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="16"/>
+      <c r="G12" s="14"/>
       <c r="H12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="J12" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="17" t="s">
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="B13" s="14"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="6">
         <v>5</v>
       </c>
@@ -1545,13 +1634,13 @@
       <c r="I13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="16"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="17"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="13"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="20" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="6">
@@ -1575,8 +1664,8 @@
       <c r="I14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="16"/>
-      <c r="K14" s="18"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="15"/>
       <c r="L14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1585,7 +1674,7 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="B15" s="14"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="6">
         <v>2</v>
       </c>
@@ -1607,7 +1696,7 @@
       <c r="I15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J15" s="16" t="s">
+      <c r="J15" s="14" t="s">
         <v>30</v>
       </c>
       <c r="K15" s="3" t="s">
@@ -1621,7 +1710,7 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="B16" s="14"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="6">
         <v>3</v>
       </c>
@@ -1643,19 +1732,19 @@
       <c r="I16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="16"/>
+      <c r="J16" s="14"/>
       <c r="K16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L16" s="11" t="s">
-        <v>32</v>
+      <c r="L16" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="M16" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="2:13">
-      <c r="B17" s="14"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="6">
         <v>4</v>
       </c>
@@ -1683,15 +1772,15 @@
       <c r="K17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L17" s="11" t="s">
-        <v>32</v>
+      <c r="L17" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="M17" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="14"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="6">
         <v>5</v>
       </c>
@@ -1704,8 +1793,8 @@
       <c r="F18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="11" t="s">
-        <v>32</v>
+      <c r="G18" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>13</v>
@@ -1719,15 +1808,15 @@
       <c r="K18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L18" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="M18" s="11" t="s">
-        <v>32</v>
+      <c r="L18" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="2:13">
-      <c r="B19" s="14"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="6">
         <v>6</v>
       </c>
@@ -1740,8 +1829,8 @@
       <c r="F19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="11" t="s">
-        <v>32</v>
+      <c r="G19" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>13</v>
@@ -1755,44 +1844,62 @@
       <c r="K19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L19" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="M19" s="11" t="s">
-        <v>32</v>
+      <c r="L19" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="2:13">
-      <c r="B20" s="14"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="6">
         <v>7</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
+      <c r="D20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" spans="2:13">
-      <c r="B21" s="14"/>
-      <c r="C21" s="6">
-        <v>8</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
     </row>
     <row r="23" spans="2:13">
       <c r="B23" s="1" t="s">
@@ -1805,14 +1912,14 @@
         <v>24</v>
       </c>
       <c r="C25" s="4">
-        <v>41794</v>
+        <v>41802</v>
       </c>
     </row>
     <row r="27" spans="2:13">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="15"/>
+      <c r="C27" s="17"/>
       <c r="D27" s="1" t="s">
         <v>2</v>
       </c>
@@ -1845,7 +1952,7 @@
       </c>
     </row>
     <row r="28" spans="2:13">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="6">
@@ -1863,7 +1970,7 @@
       <c r="M28" s="9"/>
     </row>
     <row r="29" spans="2:13">
-      <c r="B29" s="14"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="6">
         <v>2</v>
       </c>
@@ -1899,7 +2006,7 @@
       </c>
     </row>
     <row r="30" spans="2:13">
-      <c r="B30" s="14"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="6">
         <v>3</v>
       </c>
@@ -1935,7 +2042,7 @@
       </c>
     </row>
     <row r="31" spans="2:13">
-      <c r="B31" s="14"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="6">
         <v>4</v>
       </c>
@@ -1971,7 +2078,7 @@
       </c>
     </row>
     <row r="32" spans="2:13">
-      <c r="B32" s="14"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="6">
         <v>5</v>
       </c>
@@ -2007,7 +2114,7 @@
       </c>
     </row>
     <row r="33" spans="2:13">
-      <c r="B33" s="14"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="6">
         <v>6</v>
       </c>
@@ -2043,7 +2150,7 @@
       </c>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="14"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="6">
         <v>7</v>
       </c>
@@ -2079,7 +2186,7 @@
       </c>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="14"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="6">
         <v>8</v>
       </c>
@@ -2115,7 +2222,7 @@
       </c>
     </row>
     <row r="36" spans="2:13">
-      <c r="B36" s="14"/>
+      <c r="B36" s="12"/>
       <c r="C36" s="6">
         <v>9</v>
       </c>
@@ -2151,7 +2258,7 @@
       </c>
     </row>
     <row r="37" spans="2:13">
-      <c r="B37" s="14"/>
+      <c r="B37" s="12"/>
       <c r="C37" s="6">
         <v>10</v>
       </c>
@@ -2187,7 +2294,7 @@
       </c>
     </row>
     <row r="38" spans="2:13">
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C38" s="8">
@@ -2225,7 +2332,7 @@
       </c>
     </row>
     <row r="39" spans="2:13">
-      <c r="B39" s="13"/>
+      <c r="B39" s="16"/>
       <c r="C39" s="8">
         <v>2</v>
       </c>
@@ -2261,7 +2368,7 @@
       </c>
     </row>
     <row r="40" spans="2:13">
-      <c r="B40" s="13"/>
+      <c r="B40" s="16"/>
       <c r="C40" s="8">
         <v>3</v>
       </c>
@@ -2297,7 +2404,7 @@
       </c>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" s="13"/>
+      <c r="B41" s="16"/>
       <c r="C41" s="8">
         <v>4</v>
       </c>
@@ -2333,7 +2440,7 @@
       </c>
     </row>
     <row r="42" spans="2:13">
-      <c r="B42" s="13"/>
+      <c r="B42" s="16"/>
       <c r="C42" s="8">
         <v>5</v>
       </c>
@@ -2369,7 +2476,7 @@
       </c>
     </row>
     <row r="43" spans="2:13">
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C43" s="8">
@@ -2407,7 +2514,7 @@
       </c>
     </row>
     <row r="44" spans="2:13">
-      <c r="B44" s="13"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="8">
         <v>2</v>
       </c>
@@ -2443,7 +2550,7 @@
       </c>
     </row>
     <row r="45" spans="2:13">
-      <c r="B45" s="13"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="8">
         <v>3</v>
       </c>
@@ -2479,7 +2586,7 @@
       </c>
     </row>
     <row r="46" spans="2:13">
-      <c r="B46" s="13"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="8">
         <v>4</v>
       </c>
@@ -2515,7 +2622,7 @@
       </c>
     </row>
     <row r="47" spans="2:13">
-      <c r="B47" s="13"/>
+      <c r="B47" s="22"/>
       <c r="C47" s="8">
         <v>5</v>
       </c>
@@ -2551,7 +2658,7 @@
       </c>
     </row>
     <row r="48" spans="2:13">
-      <c r="B48" s="13"/>
+      <c r="B48" s="22"/>
       <c r="C48" s="8">
         <v>6</v>
       </c>
@@ -2564,8 +2671,8 @@
       <c r="F48" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G48" s="11" t="s">
-        <v>32</v>
+      <c r="G48" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="H48" s="10" t="s">
         <v>13</v>
@@ -2579,64 +2686,82 @@
       <c r="K48" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="L48" s="12" t="s">
-        <v>32</v>
+      <c r="L48" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="M48" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="49" spans="2:13">
-      <c r="B49" s="13"/>
+      <c r="B49" s="22"/>
       <c r="C49" s="8">
         <v>7</v>
       </c>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="9"/>
-      <c r="L49" s="9"/>
-      <c r="M49" s="9"/>
+      <c r="D49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J49" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M49" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="50" spans="2:13">
-      <c r="B50" s="13"/>
-      <c r="C50" s="8">
-        <v>8</v>
-      </c>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="9"/>
-      <c r="L50" s="9"/>
-      <c r="M50" s="9"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="8"/>
     </row>
   </sheetData>
   <sortState ref="D4:M4">
     <sortCondition ref="D4"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B28:B37"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="B43:B49"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B13"/>
-    <mergeCell ref="B14:B21"/>
     <mergeCell ref="M12:M13"/>
     <mergeCell ref="J12:J14"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="G10:G12"/>
     <mergeCell ref="K7:K14"/>
     <mergeCell ref="L8:L13"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="B43:B50"/>
-    <mergeCell ref="B28:B37"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="J15:J16"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>